<commit_message>
Added RPA.Excel.Files test - Reading Writing data
</commit_message>
<xml_diff>
--- a/BrowserTest/Data/LoginData.xlsx
+++ b/BrowserTest/Data/LoginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simra\Desktop\BrowserLibrary_RF\BrowserTest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E86E8B3-4D1A-47CE-83E6-58F695A0B954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFA0877-C271-42CF-9700-3FC68AF93AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{FB6C15AF-7C41-477E-8D9C-ACD2DC19F9AD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FB6C15AF-7C41-477E-8D9C-ACD2DC19F9AD}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Test4</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F756A1-C2D1-41F2-A012-820AC90AF293}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,15 +420,18 @@
     <col min="2" max="2" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -433,7 +439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -441,7 +447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -483,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6C8151-423F-430D-A691-D3234BA3CAF2}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added RPA tests for Excel Read, Write in Browser tests + bonus keywords
</commit_message>
<xml_diff>
--- a/BrowserTest/Data/LoginData.xlsx
+++ b/BrowserTest/Data/LoginData.xlsx
@@ -8,26 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simra\Desktop\BrowserLibrary_RF\BrowserTest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFA0877-C271-42CF-9700-3FC68AF93AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B1142E-FEE6-4053-80EC-4328FF9C9A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FB6C15AF-7C41-477E-8D9C-ACD2DC19F9AD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="Data1" sheetId="2" r:id="rId2"/>
-    <sheet name="Data2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -35,28 +29,34 @@
     <t>Password</t>
   </si>
   <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Test4</t>
-  </si>
-  <si>
-    <t>Result</t>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A7</t>
   </si>
 </sst>
 </file>
@@ -407,17 +407,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F756A1-C2D1-41F2-A012-820AC90AF293}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -428,7 +429,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -438,18 +439,21 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -461,53 +465,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9268C02-A22E-4594-A592-DC5B1E84322A}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="D1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6C8151-423F-430D-A691-D3234BA3CAF2}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="1" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>